<commit_message>
add coral reef data entry spreadsheets
</commit_message>
<xml_diff>
--- a/corals/final_spreadsheets/Coral Reef Demographics_marinegeo_protocol.xlsx
+++ b/corals/final_spreadsheets/Coral Reef Demographics_marinegeo_protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>definition</t>
   </si>
@@ -137,12 +137,21 @@
     <t xml:space="preserve">YYYY</t>
   </si>
   <si>
+    <t xml:space="preserve">data_entry_person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full name of data entry person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample metadata</t>
+  </si>
+  <si>
     <t xml:space="preserve">distance_completed</t>
   </si>
   <si>
-    <t xml:space="preserve">sample metadata</t>
-  </si>
-  <si>
     <t xml:space="preserve">distribution</t>
   </si>
   <si>
@@ -150,9 +159,6 @@
   </si>
   <si>
     <t xml:space="preserve">Any additional notes regarding observations, context, or concerns about the data.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
   </si>
   <si>
     <t xml:space="preserve">coral demographics data, coral condition data</t>
@@ -978,85 +984,89 @@
       <c r="A16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
+      <c r="B16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="9" t="s">
         <v>37</v>
       </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
+      <c r="C19" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
+      <c r="B21" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -1068,7 +1078,7 @@
     </row>
     <row r="23">
       <c r="A23" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1080,7 +1090,7 @@
     </row>
     <row r="24">
       <c r="A24" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1092,7 +1102,7 @@
     </row>
     <row r="25">
       <c r="A25" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -1104,34 +1114,30 @@
     </row>
     <row r="26">
       <c r="A26" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>37</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28">
@@ -1142,39 +1148,55 @@
         <v>51</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>52</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="C29" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
+      <c r="A30" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1213,7 +1235,8 @@
     <col min="5" max="5" width="13.71" hidden="0" customWidth="1"/>
     <col min="6" max="6" width="8.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="18.71" hidden="0" customWidth="1"/>
-    <col min="8" max="8" width="21.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="17.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="21.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1227,19 +1250,22 @@
         <v>21</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>47</v>
+      <c r="I1" s="11" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1285,22 +1311,22 @@
         <v>21</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>48</v>
-      </c>
       <c r="H1" s="11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J1" s="11" t="s">
         <v>14</v>
@@ -1367,40 +1393,40 @@
         <v>21</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>48</v>
-      </c>
       <c r="H1" s="11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>17</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="P1" s="11" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
update coral demographics spreadsheet
</commit_message>
<xml_diff>
--- a/corals/final_spreadsheets/Coral Reef Demographics_marinegeo_protocol.xlsx
+++ b/corals/final_spreadsheets/Coral Reef Demographics_marinegeo_protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>definition</t>
   </si>
@@ -71,25 +71,22 @@
     <t xml:space="preserve">CORAL REEF DEMOGRAPHICS</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;80</t>
+    <t xml:space="preserve">&gt;80_cm</t>
   </si>
   <si>
     <t xml:space="preserve">coral demographics data</t>
   </si>
   <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80</t>
+    <t xml:space="preserve">11-20_cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21-40_cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41-80_cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-10_cm</t>
   </si>
   <si>
     <t xml:space="preserve">condition_code</t>
@@ -164,7 +161,10 @@
     <t xml:space="preserve">coral demographics data, coral condition data</t>
   </si>
   <si>
-    <t xml:space="preserve">juveniles</t>
+    <t xml:space="preserve">isolate_1-4_cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juveniles_1-4_cm</t>
   </si>
   <si>
     <t xml:space="preserve">location_name</t>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t xml:space="preserve">percent_mortality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">predation_bites</t>
   </si>
   <si>
     <t xml:space="preserve">rate_tl</t>
@@ -887,19 +890,19 @@
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
@@ -911,89 +914,89 @@
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
+      <c r="B12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="D13" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>31</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>34</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17">
@@ -1005,35 +1008,35 @@
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
+      <c r="B18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>34</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20">
@@ -1056,12 +1059,12 @@
         <v>43</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22">
@@ -1073,7 +1076,7 @@
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23">
@@ -1085,7 +1088,7 @@
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24">
@@ -1097,7 +1100,7 @@
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25">
@@ -1109,7 +1112,7 @@
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26">
@@ -1121,23 +1124,19 @@
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28">
@@ -1145,58 +1144,74 @@
         <v>50</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="C29" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>54</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
+      <c r="A31" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1241,31 +1256,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>42</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1290,64 +1305,68 @@
     <col min="6" max="6" width="8.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="15.71" hidden="0" customWidth="1"/>
     <col min="8" max="8" width="20.71" hidden="0" customWidth="1"/>
-    <col min="9" max="9" width="9.71" hidden="0" customWidth="1"/>
-    <col min="10" max="10" width="3.71" hidden="0" customWidth="1"/>
-    <col min="11" max="11" width="3.71" hidden="0" customWidth="1"/>
-    <col min="12" max="12" width="3.71" hidden="0" customWidth="1"/>
-    <col min="13" max="13" width="3.71" hidden="0" customWidth="1"/>
-    <col min="14" max="14" width="3.71" hidden="0" customWidth="1"/>
-    <col min="15" max="15" width="6.71" hidden="0" customWidth="1"/>
-    <col min="16" max="16" width="24.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="16.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="14.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="7.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="8.71" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="8.71" hidden="0" customWidth="1"/>
+    <col min="14" max="14" width="8.71" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="9.71" hidden="0" customWidth="1"/>
+    <col min="16" max="16" width="15.71" hidden="0" customWidth="1"/>
+    <col min="17" max="17" width="24.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>42</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>41</v>
       </c>
       <c r="J1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="O1" s="11" t="s">
         <v>10</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>20</v>
+        <v>48</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1384,28 +1403,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>42</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>44</v>
@@ -1417,19 +1436,19 @@
         <v>47</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M1" s="11" t="s">
         <v>46</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>